<commit_message>
Did a whole bunch of stuff - made provisional planning - changed the test application - added the casus
</commit_message>
<xml_diff>
--- a/Activiteitenplanning Project-Groepje 7.xlsx
+++ b/Activiteitenplanning Project-Groepje 7.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somebody\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joris\Documents\HBO-ICT\Jaar 1\Periode 4 echt\DBJavaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,91 +24,130 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Activiteit</t>
   </si>
   <si>
-    <t>Duur</t>
-  </si>
-  <si>
     <t>Afhankelijk van</t>
   </si>
   <si>
     <t>EER-Model maken</t>
   </si>
   <si>
-    <t>Database maken</t>
-  </si>
-  <si>
-    <t>Klassen maken met properties</t>
-  </si>
-  <si>
-    <t>Database koppelen aan applicatie</t>
-  </si>
-  <si>
-    <t>Begint</t>
-  </si>
-  <si>
     <t>Activiteit nummer</t>
   </si>
   <si>
-    <t>Werken aan graphische gedeelte van applicatie</t>
-  </si>
-  <si>
-    <t>Testen en puntjes op de i zetten</t>
-  </si>
-  <si>
-    <t>week 3</t>
-  </si>
-  <si>
-    <t>1 week</t>
-  </si>
-  <si>
-    <t>week 4</t>
-  </si>
-  <si>
     <t>Activiteit 1</t>
   </si>
   <si>
-    <t>week 5</t>
-  </si>
-  <si>
-    <t>week 8</t>
-  </si>
-  <si>
-    <t>week 6 en 7</t>
-  </si>
-  <si>
-    <t>2 weken</t>
-  </si>
-  <si>
     <t>Activiteit 2</t>
   </si>
   <si>
-    <t>Activiteit 3 en 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t>Activiteit 3</t>
-  </si>
-  <si>
     <t>Activiteit 4</t>
   </si>
   <si>
-    <t>Activiteit 5</t>
-  </si>
-  <si>
-    <t>Activiteit 6</t>
+    <t>RRM-Model maken</t>
+  </si>
+  <si>
+    <t>RIM-Model maken</t>
+  </si>
+  <si>
+    <t>Start op</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Database aanmaken</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Queries opstellen</t>
+  </si>
+  <si>
+    <t>Tabel Student maken</t>
+  </si>
+  <si>
+    <t>Tabel School maken</t>
+  </si>
+  <si>
+    <t>Tabel Bedrijf maken</t>
+  </si>
+  <si>
+    <t>Tabel Contactpersoon maken</t>
+  </si>
+  <si>
+    <t>Tabel Traject (+ onderliggende) maken</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Zoektab implementeren</t>
+  </si>
+  <si>
+    <t>Views bepalen</t>
+  </si>
+  <si>
+    <t>Overzichtstab implementeren</t>
+  </si>
+  <si>
+    <t>Toevoegtab implementeren</t>
+  </si>
+  <si>
+    <t>Duur (in dagen)</t>
+  </si>
+  <si>
+    <t>Testen + Testrapport opstellen</t>
+  </si>
+  <si>
+    <t>UseCase diagram maken</t>
+  </si>
+  <si>
+    <t>Use Case beschrijving maken</t>
+  </si>
+  <si>
+    <t>Activiteit 3 en 6</t>
+  </si>
+  <si>
+    <t>Joris</t>
+  </si>
+  <si>
+    <t>Stef</t>
+  </si>
+  <si>
+    <t>Marouane</t>
+  </si>
+  <si>
+    <t>Bas</t>
+  </si>
+  <si>
+    <t>Tabellen vullen met test data</t>
+  </si>
+  <si>
+    <t>Activiteit 7 t/m 11</t>
+  </si>
+  <si>
+    <t>Activiteit 7 t/m 13</t>
+  </si>
+  <si>
+    <t>Activiteit 14</t>
+  </si>
+  <si>
+    <t>Activiteit 15 t/m 17</t>
+  </si>
+  <si>
+    <t>Bas + Stef</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,14 +181,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,13 +240,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Linked Cell" xfId="1" builtinId="24"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Gekoppelde cel" xfId="1" builtinId="24"/>
+    <cellStyle name="Notitie" xfId="2" builtinId="10"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -231,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,136 +524,415 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="5" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="3" max="5" width="27.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>42508</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" s="3">
+        <f>(C2+D2)</f>
+        <v>42510</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C8" si="0">(C3+D3)</f>
+        <v>42511</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>42512</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>42513</v>
+      </c>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>42515</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>42516</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3">
+        <f>(C12+D12)</f>
+        <v>42517</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <f>(C13+D13)</f>
+        <v>42518</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <f>(C14+D14)</f>
+        <v>42519</v>
+      </c>
+      <c r="D15" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <f>(C15+D15)</f>
+        <v>42522</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C17" s="3">
+        <f>(C15+D15)</f>
+        <v>42522</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C18" s="3">
+        <f>(C15+D15)</f>
+        <v>42522</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
+      <c r="C19" s="3">
+        <f>(C18+D18)</f>
+        <v>42525</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put  back the planning
</commit_message>
<xml_diff>
--- a/Activiteitenplanning Project-Groepje 7.xlsx
+++ b/Activiteitenplanning Project-Groepje 7.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somebody\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joris\Documents\HBO-ICT\Jaar 1\Periode 4 echt\DBJavaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,91 +24,130 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Activiteit</t>
   </si>
   <si>
-    <t>Duur</t>
-  </si>
-  <si>
     <t>Afhankelijk van</t>
   </si>
   <si>
     <t>EER-Model maken</t>
   </si>
   <si>
-    <t>Database maken</t>
-  </si>
-  <si>
-    <t>Klassen maken met properties</t>
-  </si>
-  <si>
-    <t>Database koppelen aan applicatie</t>
-  </si>
-  <si>
-    <t>Begint</t>
-  </si>
-  <si>
     <t>Activiteit nummer</t>
   </si>
   <si>
-    <t>Werken aan graphische gedeelte van applicatie</t>
-  </si>
-  <si>
-    <t>Testen en puntjes op de i zetten</t>
-  </si>
-  <si>
-    <t>week 3</t>
-  </si>
-  <si>
-    <t>1 week</t>
-  </si>
-  <si>
-    <t>week 4</t>
-  </si>
-  <si>
     <t>Activiteit 1</t>
   </si>
   <si>
-    <t>week 5</t>
-  </si>
-  <si>
-    <t>week 8</t>
-  </si>
-  <si>
-    <t>week 6 en 7</t>
-  </si>
-  <si>
-    <t>2 weken</t>
-  </si>
-  <si>
     <t>Activiteit 2</t>
   </si>
   <si>
-    <t>Activiteit 3 en 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t>Activiteit 3</t>
-  </si>
-  <si>
     <t>Activiteit 4</t>
   </si>
   <si>
-    <t>Activiteit 5</t>
-  </si>
-  <si>
-    <t>Activiteit 6</t>
+    <t>RRM-Model maken</t>
+  </si>
+  <si>
+    <t>RIM-Model maken</t>
+  </si>
+  <si>
+    <t>Start op</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Database aanmaken</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Queries opstellen</t>
+  </si>
+  <si>
+    <t>Tabel Student maken</t>
+  </si>
+  <si>
+    <t>Tabel School maken</t>
+  </si>
+  <si>
+    <t>Tabel Bedrijf maken</t>
+  </si>
+  <si>
+    <t>Tabel Contactpersoon maken</t>
+  </si>
+  <si>
+    <t>Tabel Traject (+ onderliggende) maken</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Zoektab implementeren</t>
+  </si>
+  <si>
+    <t>Views bepalen</t>
+  </si>
+  <si>
+    <t>Overzichtstab implementeren</t>
+  </si>
+  <si>
+    <t>Toevoegtab implementeren</t>
+  </si>
+  <si>
+    <t>Duur (in dagen)</t>
+  </si>
+  <si>
+    <t>Testen + Testrapport opstellen</t>
+  </si>
+  <si>
+    <t>UseCase diagram maken</t>
+  </si>
+  <si>
+    <t>Use Case beschrijving maken</t>
+  </si>
+  <si>
+    <t>Activiteit 3 en 6</t>
+  </si>
+  <si>
+    <t>Joris</t>
+  </si>
+  <si>
+    <t>Stef</t>
+  </si>
+  <si>
+    <t>Marouane</t>
+  </si>
+  <si>
+    <t>Bas</t>
+  </si>
+  <si>
+    <t>Tabellen vullen met test data</t>
+  </si>
+  <si>
+    <t>Activiteit 7 t/m 11</t>
+  </si>
+  <si>
+    <t>Activiteit 7 t/m 13</t>
+  </si>
+  <si>
+    <t>Activiteit 14</t>
+  </si>
+  <si>
+    <t>Activiteit 15 t/m 17</t>
+  </si>
+  <si>
+    <t>Bas + Stef</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,14 +181,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,13 +240,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Linked Cell" xfId="1" builtinId="24"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Gekoppelde cel" xfId="1" builtinId="24"/>
+    <cellStyle name="Notitie" xfId="2" builtinId="10"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -231,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,136 +524,415 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="5" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="3" max="5" width="27.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>42508</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" s="3">
+        <f>(C2+D2)</f>
+        <v>42510</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C8" si="0">(C3+D3)</f>
+        <v>42511</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>42512</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>42513</v>
+      </c>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>42515</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>42516</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <f>(C7+D7)</f>
+        <v>42516</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3">
+        <f>(C12+D12)</f>
+        <v>42517</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <f>(C13+D13)</f>
+        <v>42518</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <f>(C14+D14)</f>
+        <v>42519</v>
+      </c>
+      <c r="D15" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <f>(C15+D15)</f>
+        <v>42522</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C17" s="3">
+        <f>(C15+D15)</f>
+        <v>42522</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C18" s="3">
+        <f>(C15+D15)</f>
+        <v>42522</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
+      <c r="C19" s="3">
+        <f>(C18+D18)</f>
+        <v>42525</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the EER Model with double lines and with "inschrijving"
</commit_message>
<xml_diff>
--- a/Activiteitenplanning Project-Groepje 7.xlsx
+++ b/Activiteitenplanning Project-Groepje 7.xlsx
@@ -98,9 +98,6 @@
     <t>Toevoegtab implementeren</t>
   </si>
   <si>
-    <t>Duur (in dagen)</t>
-  </si>
-  <si>
     <t>Testen + Testrapport opstellen</t>
   </si>
   <si>
@@ -141,20 +138,16 @@
   </si>
   <si>
     <t>Bas + Stef</t>
+  </si>
+  <si>
+    <t>Duur (dagen)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,13 +158,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,11 +181,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -216,36 +203,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Gekoppelde cel" xfId="1" builtinId="24"/>
-    <cellStyle name="Notitie" xfId="2" builtinId="10"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,15 +498,17 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
-    <col min="3" max="5" width="27.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -549,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -559,274 +532,274 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>42508</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>29</v>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f>(C2+D2)</f>
         <v>42510</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:C8" si="0">(C3+D3)</f>
         <v>42511</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>42512</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>42513</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>31</v>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>42515</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>42516</v>
       </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f>(C7+D7)</f>
         <v>42516</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <f>(C7+D7)</f>
         <v>42516</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f>(C7+D7)</f>
         <v>42516</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <f>(C7+D7)</f>
         <v>42516</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2">
         <f>(C12+D12)</f>
         <v>42517</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <f>(C13+D13)</f>
         <v>42518</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -834,105 +807,105 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f>(C14+D14)</f>
         <v>42519</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <f>(C15+D15)</f>
         <v>42522</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" t="s">
-        <v>29</v>
+      <c r="E16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <f>(C15+D15)</f>
         <v>42522</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <f>(C15+D15)</f>
         <v>42522</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" t="s">
-        <v>31</v>
+      <c r="E18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2">
         <f>(C18+D18)</f>
         <v>42525</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>3</v>
       </c>
       <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
         <v>37</v>
-      </c>
-      <c r="F19" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the last details to EER. IT. IS. DONE!!!!!!
</commit_message>
<xml_diff>
--- a/Activiteitenplanning Project-Groepje 7.xlsx
+++ b/Activiteitenplanning Project-Groepje 7.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Activiteit</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Duur (dagen)</t>
+  </si>
+  <si>
+    <t>Marouane + Joris</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +511,7 @@
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -632,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
minor changes to app
</commit_message>
<xml_diff>
--- a/Activiteitenplanning Project-Groepje 7.xlsx
+++ b/Activiteitenplanning Project-Groepje 7.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Activiteit</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Marouane + Joris</t>
+  </si>
+  <si>
+    <t>Inschrijftab implementeren</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,19 +898,30 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <f>(C18+D18)</f>
         <v>42525</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>3</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>